<commit_message>
update database,created dll and main form
Update database and created dll references with ADO and than added main form
</commit_message>
<xml_diff>
--- a/MainDealerDatabaseDiagram.xlsx
+++ b/MainDealerDatabaseDiagram.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Main And Sub Dealer Diagram" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
   <si>
     <t>UserID</t>
   </si>
@@ -40,9 +40,6 @@
     <t>DealerMail</t>
   </si>
   <si>
-    <t>DealerType</t>
-  </si>
-  <si>
     <t>GoldBike</t>
   </si>
   <si>
@@ -74,13 +71,290 @@
   </si>
   <si>
     <t>SUB DEALERS</t>
+  </si>
+  <si>
+    <t>CATEGORIES</t>
+  </si>
+  <si>
+    <t>PRODUCTS</t>
+  </si>
+  <si>
+    <t>BRANDS</t>
+  </si>
+  <si>
+    <t>BrandID</t>
+  </si>
+  <si>
+    <t>BrandName</t>
+  </si>
+  <si>
+    <t>BrandIDFK</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>Bianchi</t>
+  </si>
+  <si>
+    <t>Colnago</t>
+  </si>
+  <si>
+    <t>Wilier Triestina</t>
+  </si>
+  <si>
+    <t>Olympia</t>
+  </si>
+  <si>
+    <t>Sram</t>
+  </si>
+  <si>
+    <t>Shimano</t>
+  </si>
+  <si>
+    <t>Trek</t>
+  </si>
+  <si>
+    <t>Cannondale</t>
+  </si>
+  <si>
+    <t>Specialized</t>
+  </si>
+  <si>
+    <t>S-Works</t>
+  </si>
+  <si>
+    <t>Derrailleurs</t>
+  </si>
+  <si>
+    <t>Cassettes</t>
+  </si>
+  <si>
+    <t>Bottom Brackets</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>QuantityPerUnit</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
+  </si>
+  <si>
+    <t>UnitsInStock</t>
+  </si>
+  <si>
+    <t>UnitsOnOrder</t>
+  </si>
+  <si>
+    <t>ReorderLevel</t>
+  </si>
+  <si>
+    <t>Discontinued</t>
+  </si>
+  <si>
+    <t>IsDeleted</t>
+  </si>
+  <si>
+    <t>DUB Press Fit 30</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>The new SRAM DUB™ bottom bracket series has a simple job-connect your crankarms and protect the smooth, long-lasting application of power to your drivetrain. To allow that singular focus, we´ve engineered the DUB™ spindle to be the one true unifying component. One oversized spindle to work across every bottom bracket standard. For better crankarm compatibility. For better protection from the elements. For longer-lasting performance. To be stronger, smoother, simpler. Now, back to the ride.</t>
+  </si>
+  <si>
+    <t>Image name</t>
+  </si>
+  <si>
+    <t>Sram XX1 Eagle XG-1299 Cassette
+Specifications:
+- Material 1-11 sprocket: Steel
+- End pinion material: Aluminum
+- Technology: X-Dome
+- Gears: 12
+- Gradation: 10-12-14-16-18-21-24-28-32-36-42-52
+- Translation bandwidth: 520%
+- Compatibility freewheel: 11-, 12-speed Sram Xd Mtb
+- Drive compatibility: Sram 12-speed drives
+- Weight: approx. 370g</t>
+  </si>
+  <si>
+    <t>Sram XX1 Eagle/X01 Eagle XG-1299</t>
+  </si>
+  <si>
+    <t>Shimano 105 R7000 DM</t>
+  </si>
+  <si>
+    <t>Oriented on the design and functionality of the top groups Ultegra and Dura-Ace. This Shimano 105 FD-R7000-F front derailleur is orientated among other things by the space that you have for wider tires, and the integration of the cable clamping and the setting via a 2 mm Allen key.
+Specifications:
+- Down-Swing
+- 11-/2-speed compatible
+- Mount: Weld-On
+- Largest chainring max. 46 - 53 teeth
+- Capacity: 16 teeth
+- Chain Line: 43.5 mm
+- Angle Rear Chainstay: 61° - 66°
+- Weight: approx. 93 g</t>
+  </si>
+  <si>
+    <t>SEND TO SUB DEALERS</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>CategoryIDFK</t>
+  </si>
+  <si>
+    <t>ProductIDFK</t>
+  </si>
+  <si>
+    <t>SubDealerIDFK</t>
+  </si>
+  <si>
+    <t>SendID</t>
+  </si>
+  <si>
+    <t>UserType</t>
+  </si>
+  <si>
+    <t>SendDate</t>
+  </si>
+  <si>
+    <t>SendQuantity</t>
+  </si>
+  <si>
+    <t>TotalPrice</t>
+  </si>
+  <si>
+    <t>Via Ludovico il Moro 22</t>
+  </si>
+  <si>
+    <t>Bergamo</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Strada Provinciale 124</t>
+  </si>
+  <si>
+    <t>Reggio Emilia</t>
+  </si>
+  <si>
+    <t>Via Monte Bianco 34</t>
+  </si>
+  <si>
+    <t>Torino</t>
+  </si>
+  <si>
+    <t>Product Unit Price * Send Quantity</t>
+  </si>
+  <si>
+    <t>SettingID</t>
+  </si>
+  <si>
+    <t>MAIN DEALER SETTINGS</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Cheiti</t>
+  </si>
+  <si>
+    <t>Strada Statale 524</t>
+  </si>
+  <si>
+    <t>SettingIDFK</t>
+  </si>
+  <si>
+    <t>LEVEL INTEGRATION ORDERS</t>
+  </si>
+  <si>
+    <t>LevelIntegrationID</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Completion Level</t>
+  </si>
+  <si>
+    <t>Order Completion Date</t>
+  </si>
+  <si>
+    <t>DiscountID</t>
+  </si>
+  <si>
+    <t>DiscountType</t>
+  </si>
+  <si>
+    <t>DealerType(DiscountIDFK)</t>
+  </si>
+  <si>
+    <t>DISCOUNT RATES SETTINGS</t>
+  </si>
+  <si>
+    <t>InvoiceTaxAmount</t>
+  </si>
+  <si>
+    <t>DealerCountry</t>
+  </si>
+  <si>
+    <t>DealerPostalCode</t>
+  </si>
+  <si>
+    <t>DealerCity</t>
+  </si>
+  <si>
+    <t>DealerAddress</t>
+  </si>
+  <si>
+    <t>DiscountAmount</t>
+  </si>
+  <si>
+    <t>SubTotalPrice</t>
+  </si>
+  <si>
+    <t>Tax(InvoiceTaxAmount)</t>
+  </si>
+  <si>
+    <t>(SubTotalPrice * Tax)/100</t>
+  </si>
+  <si>
+    <t>SubTotalPrice+Tax</t>
+  </si>
+  <si>
+    <t>Cavallo Del Vento</t>
+  </si>
+  <si>
+    <t>cavallodelvento@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,8 +370,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,7 +392,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CC00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,31 +504,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -215,6 +603,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF99CC00"/>
+      <color rgb="FFFF3399"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -489,134 +883,944 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="11">
+        <v>66022</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1881</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
+        <v>1</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
+        <v>2</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
+        <v>3</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>1</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="6">
+        <v>24100</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="17">
+        <v>2</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="6">
+        <v>42100</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
-        <v>1881</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E4" s="4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E5" s="4">
+      <c r="D19" s="17">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>15</v>
+      <c r="E19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="6">
+        <v>10100</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:H1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
-    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="C17" r:id="rId1"/>
+    <hyperlink ref="C18" r:id="rId2"/>
+    <hyperlink ref="C19" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="D1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="H1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="28"/>
+    </row>
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="13">
+        <v>1</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="13">
+        <v>1</v>
+      </c>
+      <c r="O3" s="13">
+        <v>1354.99</v>
+      </c>
+      <c r="P3" s="13">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="13">
+        <v>0</v>
+      </c>
+      <c r="R3" s="13">
+        <v>15</v>
+      </c>
+      <c r="S3" s="13">
+        <v>1</v>
+      </c>
+      <c r="T3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="13">
+        <v>2</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="13">
+        <v>1</v>
+      </c>
+      <c r="O4" s="13">
+        <v>16009.99</v>
+      </c>
+      <c r="P4" s="13">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>30</v>
+      </c>
+      <c r="R4" s="13">
+        <v>20</v>
+      </c>
+      <c r="S4" s="13">
+        <v>0</v>
+      </c>
+      <c r="T4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2">
+        <v>6</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3</v>
+      </c>
+      <c r="J5" s="13">
+        <v>3</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" s="13">
+        <v>1</v>
+      </c>
+      <c r="O5" s="13">
+        <v>1210.95</v>
+      </c>
+      <c r="P5" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>15</v>
+      </c>
+      <c r="R5" s="13">
+        <v>0</v>
+      </c>
+      <c r="S5" s="13">
+        <v>0</v>
+      </c>
+      <c r="T5" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+    </row>
+    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="13">
+        <v>1</v>
+      </c>
+      <c r="K9" s="11">
+        <v>1</v>
+      </c>
+      <c r="L9" s="6">
+        <v>1</v>
+      </c>
+      <c r="M9" s="8">
+        <v>1</v>
+      </c>
+      <c r="N9" s="9">
+        <v>45766</v>
+      </c>
+      <c r="O9" s="8">
+        <v>1</v>
+      </c>
+      <c r="P9" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2</v>
+      </c>
+      <c r="J10" s="13">
+        <v>2</v>
+      </c>
+      <c r="K10" s="11">
+        <v>1</v>
+      </c>
+      <c r="L10" s="6">
+        <v>1</v>
+      </c>
+      <c r="M10" s="8">
+        <v>2</v>
+      </c>
+      <c r="N10" s="9">
+        <v>45766</v>
+      </c>
+      <c r="O10" s="8">
+        <v>2</v>
+      </c>
+      <c r="P10" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="T10" s="10"/>
+    </row>
+    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="2">
+        <v>6</v>
+      </c>
+      <c r="I11" s="4">
+        <v>3</v>
+      </c>
+      <c r="J11" s="13">
+        <v>3</v>
+      </c>
+      <c r="K11" s="11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6">
+        <v>3</v>
+      </c>
+      <c r="M11" s="8">
+        <v>3</v>
+      </c>
+      <c r="N11" s="9">
+        <v>45768</v>
+      </c>
+      <c r="O11" s="8">
+        <v>1</v>
+      </c>
+      <c r="P11" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="T11" s="10"/>
+    </row>
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2</v>
+      </c>
+      <c r="J12" s="13">
+        <v>2</v>
+      </c>
+      <c r="K12" s="11">
+        <v>1</v>
+      </c>
+      <c r="L12" s="6">
+        <v>2</v>
+      </c>
+      <c r="M12" s="8">
+        <v>4</v>
+      </c>
+      <c r="N12" s="9">
+        <v>45769</v>
+      </c>
+      <c r="O12" s="8">
+        <v>3</v>
+      </c>
+      <c r="P12" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="T12" s="10"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H15" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H16" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="8:15" x14ac:dyDescent="0.3">
+      <c r="H17" s="15">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
+        <v>5</v>
+      </c>
+      <c r="J17" s="4">
+        <v>2</v>
+      </c>
+      <c r="K17" s="13">
+        <v>2</v>
+      </c>
+      <c r="L17" s="15">
+        <f>Q4</f>
+        <v>30</v>
+      </c>
+      <c r="M17" s="16">
+        <v>45758</v>
+      </c>
+      <c r="N17" s="15">
+        <v>30</v>
+      </c>
+      <c r="O17" s="16">
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="18" spans="8:15" x14ac:dyDescent="0.3">
+      <c r="H18" s="15">
+        <v>2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>6</v>
+      </c>
+      <c r="J18" s="4">
+        <v>3</v>
+      </c>
+      <c r="K18" s="13">
+        <v>3</v>
+      </c>
+      <c r="L18" s="15">
+        <f>Q5</f>
+        <v>15</v>
+      </c>
+      <c r="M18" s="16">
+        <v>45766</v>
+      </c>
+      <c r="N18" s="15">
+        <v>10</v>
+      </c>
+      <c r="O18" s="16">
+        <v>45769</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="H1:T1"/>
+    <mergeCell ref="H15:O15"/>
+    <mergeCell ref="H7:T7"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Menu Strip Items Added to Main Form
</commit_message>
<xml_diff>
--- a/MainDealerDatabaseDiagram.xlsx
+++ b/MainDealerDatabaseDiagram.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="110">
   <si>
     <t>UserID</t>
   </si>
@@ -348,6 +348,27 @@
   </si>
   <si>
     <t>cavallodelvento@gmail.com</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>nasuh</t>
+  </si>
+  <si>
+    <t>nazurabi</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Write when If deleted or edited order vb information</t>
+  </si>
+  <si>
+    <t>Image Name</t>
   </si>
 </sst>
 </file>
@@ -439,7 +460,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -499,12 +520,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -533,30 +563,30 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -590,11 +620,20 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -883,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,7 +947,7 @@
     <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>74</v>
       </c>
@@ -919,68 +958,76 @@
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>66022</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="10">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -993,199 +1040,235 @@
       <c r="D6" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E6" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="C7" s="5">
-        <v>1881</v>
+        <v>1863</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="E7" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1234</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
-        <v>1</v>
-      </c>
-      <c r="B11" s="17" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>1</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C12" s="16">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="17">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
         <v>2</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C13" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
         <v>3</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C14" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
-        <v>1</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="I17" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G18" s="6">
         <v>24100</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
-        <v>2</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="17">
-        <v>2</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="6">
-        <v>42100</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="17">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="D19" s="16">
+        <v>2</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G19" s="6">
-        <v>10100</v>
+        <v>42100</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>67</v>
       </c>
+      <c r="I19" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="16">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="6">
+        <v>10100</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C17" r:id="rId1"/>
-    <hyperlink ref="C18" r:id="rId2"/>
-    <hyperlink ref="C19" r:id="rId3"/>
+    <hyperlink ref="C18" r:id="rId1"/>
+    <hyperlink ref="C19" r:id="rId2"/>
+    <hyperlink ref="C20" r:id="rId3"/>
     <hyperlink ref="C3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1195,53 +1278,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" style="1" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" style="1" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="24"/>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="F1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="H1" s="26" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="L1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
       <c r="O1" s="27"/>
@@ -1249,576 +1335,688 @@
       <c r="Q1" s="27"/>
       <c r="R1" s="27"/>
       <c r="S1" s="27"/>
-      <c r="T1" s="28"/>
-    </row>
-    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="28"/>
+    </row>
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="N2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="O2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="P2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="Q2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="R2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="S2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="T2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="U2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="V2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="W2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="X2" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="2">
         <v>5</v>
       </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="2">
         <v>5</v>
       </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="13">
-        <v>1</v>
-      </c>
-      <c r="K3" s="13" t="s">
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="12">
+        <v>1</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="P3" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="Q3" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="13">
-        <v>1</v>
-      </c>
-      <c r="O3" s="13">
+      <c r="R3" s="12">
+        <v>1</v>
+      </c>
+      <c r="S3" s="12">
         <v>1354.99</v>
       </c>
-      <c r="P3" s="13">
+      <c r="T3" s="12">
         <v>10</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="U3" s="12">
         <v>0</v>
       </c>
-      <c r="R3" s="13">
+      <c r="V3" s="12">
         <v>15</v>
       </c>
-      <c r="S3" s="13">
-        <v>1</v>
-      </c>
-      <c r="T3" s="13">
+      <c r="W3" s="12">
+        <v>1</v>
+      </c>
+      <c r="X3" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="2">
         <v>5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="G4" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" s="2">
         <v>5</v>
       </c>
-      <c r="I4" s="4">
+      <c r="M4" s="4">
         <v>2</v>
       </c>
-      <c r="J4" s="13">
+      <c r="N4" s="12">
         <v>2</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="O4" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="P4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="Q4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="13">
-        <v>1</v>
-      </c>
-      <c r="O4" s="13">
+      <c r="R4" s="12">
+        <v>1</v>
+      </c>
+      <c r="S4" s="12">
         <v>16009.99</v>
       </c>
-      <c r="P4" s="13">
+      <c r="T4" s="12">
         <v>15</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="U4" s="12">
         <v>30</v>
       </c>
-      <c r="R4" s="13">
+      <c r="V4" s="12">
         <v>20</v>
       </c>
-      <c r="S4" s="13">
+      <c r="W4" s="12">
         <v>0</v>
       </c>
-      <c r="T4" s="13">
+      <c r="X4" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="2">
         <v>6</v>
       </c>
-      <c r="E5" s="4">
+      <c r="G5" s="4">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5" s="2">
         <v>6</v>
       </c>
-      <c r="I5" s="4">
+      <c r="M5" s="4">
         <v>3</v>
       </c>
-      <c r="J5" s="13">
+      <c r="N5" s="12">
         <v>3</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="O5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="P5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="Q5" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="N5" s="13">
-        <v>1</v>
-      </c>
-      <c r="O5" s="13">
+      <c r="R5" s="12">
+        <v>1</v>
+      </c>
+      <c r="S5" s="12">
         <v>1210.95</v>
       </c>
-      <c r="P5" s="13">
+      <c r="T5" s="12">
         <v>5</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="U5" s="12">
         <v>15</v>
       </c>
-      <c r="R5" s="13">
+      <c r="V5" s="12">
         <v>0</v>
       </c>
-      <c r="S5" s="13">
+      <c r="W5" s="12">
         <v>0</v>
       </c>
-      <c r="T5" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X5" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="C7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-    </row>
-    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+    </row>
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="N8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="O8" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="P8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="Q8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="R8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="S8" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="P8" s="30" t="s">
+      <c r="T8" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="11" t="s">
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="T8" s="10" t="s">
+      <c r="X8" s="17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y8" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="2">
+      <c r="C9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" s="2">
         <v>5</v>
       </c>
-      <c r="I9" s="4">
-        <v>1</v>
-      </c>
-      <c r="J9" s="13">
-        <v>1</v>
-      </c>
-      <c r="K9" s="11">
-        <v>1</v>
-      </c>
-      <c r="L9" s="6">
-        <v>1</v>
-      </c>
-      <c r="M9" s="8">
-        <v>1</v>
-      </c>
-      <c r="N9" s="9">
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="12">
+        <v>1</v>
+      </c>
+      <c r="O9" s="10">
+        <v>1</v>
+      </c>
+      <c r="P9" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>1</v>
+      </c>
+      <c r="R9" s="9">
         <v>45766</v>
       </c>
-      <c r="O9" s="8">
-        <v>1</v>
-      </c>
-      <c r="P9" s="30" t="s">
+      <c r="S9" s="8">
+        <v>1</v>
+      </c>
+      <c r="T9" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="11" t="s">
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="T9" s="10" t="s">
+      <c r="X9" s="17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y9" s="30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="2">
+      <c r="C10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L10" s="2">
         <v>5</v>
       </c>
-      <c r="I10" s="4">
+      <c r="M10" s="4">
         <v>2</v>
       </c>
-      <c r="J10" s="13">
+      <c r="N10" s="12">
         <v>2</v>
       </c>
-      <c r="K10" s="11">
-        <v>1</v>
-      </c>
-      <c r="L10" s="6">
-        <v>1</v>
-      </c>
-      <c r="M10" s="8">
+      <c r="O10" s="10">
+        <v>1</v>
+      </c>
+      <c r="P10" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="8">
         <v>2</v>
       </c>
-      <c r="N10" s="9">
+      <c r="R10" s="9">
         <v>45766</v>
       </c>
-      <c r="O10" s="8">
+      <c r="S10" s="8">
         <v>2</v>
       </c>
-      <c r="P10" s="30" t="s">
+      <c r="T10" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="11" t="s">
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="T10" s="10"/>
-    </row>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+    </row>
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="2">
+      <c r="C11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L11" s="2">
         <v>6</v>
       </c>
-      <c r="I11" s="4">
+      <c r="M11" s="4">
         <v>3</v>
       </c>
-      <c r="J11" s="13">
+      <c r="N11" s="12">
         <v>3</v>
       </c>
-      <c r="K11" s="11">
-        <v>1</v>
-      </c>
-      <c r="L11" s="6">
+      <c r="O11" s="10">
+        <v>1</v>
+      </c>
+      <c r="P11" s="6">
         <v>3</v>
       </c>
-      <c r="M11" s="8">
+      <c r="Q11" s="8">
         <v>3</v>
       </c>
-      <c r="N11" s="9">
+      <c r="R11" s="9">
         <v>45768</v>
       </c>
-      <c r="O11" s="8">
-        <v>1</v>
-      </c>
-      <c r="P11" s="30" t="s">
+      <c r="S11" s="8">
+        <v>1</v>
+      </c>
+      <c r="T11" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="11" t="s">
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="T11" s="10"/>
-    </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+    </row>
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="2">
+      <c r="C12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12" s="2">
         <v>5</v>
       </c>
-      <c r="I12" s="4">
+      <c r="M12" s="4">
         <v>2</v>
       </c>
-      <c r="J12" s="13">
+      <c r="N12" s="12">
         <v>2</v>
       </c>
-      <c r="K12" s="11">
-        <v>1</v>
-      </c>
-      <c r="L12" s="6">
+      <c r="O12" s="10">
+        <v>1</v>
+      </c>
+      <c r="P12" s="6">
         <v>2</v>
       </c>
-      <c r="M12" s="8">
+      <c r="Q12" s="8">
         <v>4</v>
       </c>
-      <c r="N12" s="9">
+      <c r="R12" s="9">
         <v>45769</v>
       </c>
-      <c r="O12" s="8">
+      <c r="S12" s="8">
         <v>3</v>
       </c>
-      <c r="P12" s="30" t="s">
+      <c r="T12" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="11" t="s">
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="T12" s="10"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="H15" s="29" t="s">
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="L15" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="H16" s="15" t="s">
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="L16" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="N16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="O16" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="P16" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="Q16" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="N16" s="15" t="s">
+      <c r="R16" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="S16" s="14" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="H17" s="15">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2">
+      <c r="T16" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="12:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="14">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2">
         <v>5</v>
       </c>
-      <c r="J17" s="4">
+      <c r="N17" s="4">
         <v>2</v>
       </c>
-      <c r="K17" s="13">
+      <c r="O17" s="12">
         <v>2</v>
       </c>
-      <c r="L17" s="15">
-        <f>Q4</f>
+      <c r="P17" s="14">
+        <f>U4</f>
         <v>30</v>
       </c>
-      <c r="M17" s="16">
+      <c r="Q17" s="15">
         <v>45758</v>
       </c>
-      <c r="N17" s="15">
+      <c r="R17" s="14">
         <v>30</v>
       </c>
-      <c r="O17" s="16">
+      <c r="S17" s="15">
         <v>45769</v>
       </c>
-    </row>
-    <row r="18" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="H18" s="15">
+      <c r="T17" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="12:20" x14ac:dyDescent="0.3">
+      <c r="L18" s="14">
         <v>2</v>
       </c>
-      <c r="I18" s="2">
+      <c r="M18" s="2">
         <v>6</v>
       </c>
-      <c r="J18" s="4">
+      <c r="N18" s="4">
         <v>3</v>
       </c>
-      <c r="K18" s="13">
+      <c r="O18" s="12">
         <v>3</v>
       </c>
-      <c r="L18" s="15">
-        <f>Q5</f>
+      <c r="P18" s="14">
+        <f>U5</f>
         <v>15</v>
       </c>
-      <c r="M18" s="16">
+      <c r="Q18" s="15">
         <v>45766</v>
       </c>
-      <c r="N18" s="15">
+      <c r="R18" s="14">
         <v>10</v>
       </c>
-      <c r="O18" s="16">
+      <c r="S18" s="15">
         <v>45769</v>
       </c>
+      <c r="T18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="H1:T1"/>
-    <mergeCell ref="H15:O15"/>
-    <mergeCell ref="H7:T7"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="L1:X1"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="L7:Y7"/>
+    <mergeCell ref="L15:T15"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
from main dealer to sub dealer xml added
</commit_message>
<xml_diff>
--- a/MainDealerDatabaseDiagram.xlsx
+++ b/MainDealerDatabaseDiagram.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main And Sub Dealer Diagram" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
   <si>
     <t>UserID</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>Image Name</t>
+  </si>
+  <si>
+    <t>MainDealerUserIDFK</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -585,32 +588,44 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,17 +638,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -924,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,17 +958,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -1019,13 +1029,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1079,11 +1089,11 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
@@ -1130,17 +1140,17 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
@@ -1278,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:AA18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,48 +1310,49 @@
     <col min="14" max="14" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17" style="1" customWidth="1"/>
     <col min="19" max="19" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="12.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="23.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.44140625" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.88671875" style="1"/>
+    <col min="24" max="24" width="23" style="1" customWidth="1"/>
+    <col min="25" max="25" width="16.77734375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.109375" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:27" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="F1" s="25" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="F1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="L1" s="26" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="L1" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="28"/>
-    </row>
-    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="32"/>
+    </row>
+    <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -1409,7 +1420,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1477,7 +1488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1545,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1613,7 +1624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1627,7 +1638,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1640,24 +1651,26 @@
       <c r="D7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="L7" s="29" t="s">
+      <c r="L7" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-    </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
+      <c r="AA7" s="33"/>
+    </row>
+    <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1685,31 +1698,39 @@
       <c r="P8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Q8" s="8" t="s">
+      <c r="Q8" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="R8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="R8" s="8" t="s">
+      <c r="S8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="S8" s="8" t="s">
+      <c r="T8" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="T8" s="29" t="s">
+      <c r="U8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="V8" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="10" t="s">
+      <c r="W8" s="34"/>
+      <c r="X8" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="X8" s="17" t="s">
+      <c r="Y8" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="Y8" s="17" t="s">
+      <c r="Z8" s="19" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA8" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1737,31 +1758,35 @@
       <c r="P9" s="6">
         <v>1</v>
       </c>
-      <c r="Q9" s="8">
-        <v>1</v>
-      </c>
-      <c r="R9" s="9">
+      <c r="Q9" s="5">
+        <v>1</v>
+      </c>
+      <c r="R9" s="8">
+        <v>1</v>
+      </c>
+      <c r="S9" s="9">
         <v>45766</v>
       </c>
-      <c r="S9" s="8">
-        <v>1</v>
-      </c>
-      <c r="T9" s="29" t="s">
+      <c r="T9" s="8">
+        <v>1</v>
+      </c>
+      <c r="U9" s="8"/>
+      <c r="V9" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="10" t="s">
+      <c r="W9" s="36"/>
+      <c r="X9" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="X9" s="17" t="s">
+      <c r="Y9" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="Y9" s="30" t="s">
+      <c r="Z9" s="17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA9" s="19"/>
+    </row>
+    <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1789,27 +1814,31 @@
       <c r="P10" s="6">
         <v>1</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="Q10" s="5">
         <v>2</v>
       </c>
-      <c r="R10" s="9">
+      <c r="R10" s="8">
+        <v>2</v>
+      </c>
+      <c r="S10" s="9">
         <v>45766</v>
       </c>
-      <c r="S10" s="8">
+      <c r="T10" s="8">
         <v>2</v>
       </c>
-      <c r="T10" s="29" t="s">
+      <c r="U10" s="8"/>
+      <c r="V10" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="10" t="s">
+      <c r="W10" s="36"/>
+      <c r="X10" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="X10" s="17"/>
-      <c r="Y10" s="17"/>
-    </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="19"/>
+    </row>
+    <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1837,27 +1866,31 @@
       <c r="P11" s="6">
         <v>3</v>
       </c>
-      <c r="Q11" s="8">
+      <c r="Q11" s="5">
+        <v>1</v>
+      </c>
+      <c r="R11" s="8">
         <v>3</v>
       </c>
-      <c r="R11" s="9">
+      <c r="S11" s="9">
         <v>45768</v>
       </c>
-      <c r="S11" s="8">
-        <v>1</v>
-      </c>
-      <c r="T11" s="29" t="s">
+      <c r="T11" s="8">
+        <v>1</v>
+      </c>
+      <c r="U11" s="8"/>
+      <c r="V11" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="10" t="s">
+      <c r="W11" s="36"/>
+      <c r="X11" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-    </row>
-    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+    </row>
+    <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1885,40 +1918,44 @@
       <c r="P12" s="6">
         <v>2</v>
       </c>
-      <c r="Q12" s="8">
+      <c r="Q12" s="5">
+        <v>1</v>
+      </c>
+      <c r="R12" s="8">
         <v>4</v>
       </c>
-      <c r="R12" s="9">
+      <c r="S12" s="9">
         <v>45769</v>
       </c>
-      <c r="S12" s="8">
+      <c r="T12" s="8">
         <v>3</v>
       </c>
-      <c r="T12" s="29" t="s">
+      <c r="U12" s="8"/>
+      <c r="V12" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="10" t="s">
+      <c r="W12" s="36"/>
+      <c r="X12" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="X12" s="17"/>
-      <c r="Y12" s="17"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="L15" s="31" t="s">
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="L15" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="L16" s="14" t="s">
         <v>83</v>
       </c>
@@ -1973,7 +2010,7 @@
       <c r="S17" s="15">
         <v>45769</v>
       </c>
-      <c r="T17" s="33" t="s">
+      <c r="T17" s="18" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2006,17 +2043,16 @@
       <c r="T18" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="L1:X1"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="T12:V12"/>
-    <mergeCell ref="L7:Y7"/>
+  <mergeCells count="9">
+    <mergeCell ref="V12:W12"/>
     <mergeCell ref="L15:T15"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="L1:X1"/>
+    <mergeCell ref="L7:AA7"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="V11:W11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>